<commit_message>
adding class 5 English poems
</commit_message>
<xml_diff>
--- a/TestReport1.xlsx
+++ b/TestReport1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="3" activeTab="7"/>
+    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="3" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="162">
   <si>
     <t>Content</t>
   </si>
@@ -2386,8 +2386,8 @@
   <sheetPr/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2445,7 +2445,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>14</v>
@@ -2454,16 +2454,19 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>16</v>
@@ -2472,13 +2475,16 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4122,7 +4128,7 @@
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated class 6 english poems
</commit_message>
<xml_diff>
--- a/TestReport1.xlsx
+++ b/TestReport1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="3" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="2" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="173">
   <si>
     <t>Content</t>
   </si>
@@ -274,6 +274,9 @@
     <t>Gida mara</t>
   </si>
   <si>
+    <t>Initial version</t>
+  </si>
+  <si>
     <t>swathanthraya hanathe</t>
   </si>
   <si>
@@ -311,6 +314,36 @@
   </si>
   <si>
     <t>Janapada</t>
+  </si>
+  <si>
+    <t>2nd language English Poems</t>
+  </si>
+  <si>
+    <t>The elephants</t>
+  </si>
+  <si>
+    <t>IR 1.0</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>Tamarind</t>
+  </si>
+  <si>
+    <t>Believe</t>
+  </si>
+  <si>
+    <t>The Cow</t>
+  </si>
+  <si>
+    <t>Results and Roses</t>
+  </si>
+  <si>
+    <t>Paper boats</t>
+  </si>
+  <si>
+    <t>My land</t>
   </si>
   <si>
     <t>Mangala grahadalli putti</t>
@@ -1165,7 +1198,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1183,6 +1216,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2002,7 +2038,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -2011,7 +2047,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:3">
@@ -2020,7 +2056,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
@@ -2029,7 +2065,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:3">
@@ -2038,7 +2074,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:3">
@@ -2047,7 +2083,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:3">
@@ -2056,7 +2092,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:3">
@@ -2065,7 +2101,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:3">
@@ -2076,7 +2112,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:3">
@@ -2085,7 +2121,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:3">
@@ -2094,7 +2130,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:3">
@@ -2103,7 +2139,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:3">
@@ -2112,7 +2148,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:3">
@@ -2121,7 +2157,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="2:3">
@@ -2129,12 +2165,12 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2312,56 +2348,56 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="34.8" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" ht="27.6" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E4" s="2">
         <v>2.1</v>
@@ -2372,7 +2408,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +2423,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:G5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2524,13 +2560,13 @@
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="4"/>
@@ -2730,7 +2766,7 @@
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="12" customFormat="1" spans="1:6">
       <c r="A12" s="4" t="s">
@@ -2825,13 +2861,13 @@
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:1">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
     </row>
     <row r="18" customFormat="1" spans="1:1">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
     </row>
     <row r="19" customFormat="1" spans="1:1">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2998,7 +3034,7 @@
       <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="12" customFormat="1" spans="1:6">
       <c r="A12" s="4" t="s">
@@ -3093,7 +3129,7 @@
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:6">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="C17" t="s">
         <v>58</v>
       </c>
@@ -3108,7 +3144,7 @@
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:6">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="C18" t="s">
         <v>59</v>
       </c>
@@ -3123,7 +3159,7 @@
       </c>
     </row>
     <row r="19" customFormat="1" spans="1:1">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3305,7 +3341,7 @@
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="12" customFormat="1" spans="1:6">
       <c r="A12" s="4" t="s">
@@ -3400,7 +3436,7 @@
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:6">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -3418,7 +3454,7 @@
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:6">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -3436,7 +3472,7 @@
       </c>
     </row>
     <row r="19" customFormat="1" spans="1:6">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -3483,10 +3519,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -3521,7 +3557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="1" spans="1:7">
+    <row r="3" customFormat="1" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -3543,14 +3579,17 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" customFormat="1" spans="1:7">
+      <c r="H3" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:8">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -3564,14 +3603,15 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" customFormat="1" spans="1:7">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" customFormat="1" spans="1:8">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -3585,14 +3625,15 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="1" spans="1:7">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" customFormat="1" spans="1:8">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -3606,14 +3647,15 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" customFormat="1" spans="1:6">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" customFormat="1" spans="1:8">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -3624,14 +3666,15 @@
       <c r="F7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" customFormat="1" spans="1:7">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" customFormat="1" spans="1:8">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -3645,14 +3688,15 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" customFormat="1" spans="1:7">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" customFormat="1" spans="1:8">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -3666,14 +3710,15 @@
       <c r="G9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" customFormat="1" spans="1:7">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" customFormat="1" spans="1:8">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -3687,8 +3732,9 @@
       <c r="G10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" customFormat="1" spans="1:7">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="12" customFormat="1" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -3696,7 +3742,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -3710,14 +3756,17 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" customFormat="1" spans="1:7">
+      <c r="H12" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" spans="1:8">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -3731,14 +3780,15 @@
       <c r="G13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" customFormat="1" spans="1:7">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" customFormat="1" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -3752,14 +3802,15 @@
       <c r="G14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="1" spans="1:7">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" customFormat="1" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -3773,14 +3824,15 @@
       <c r="G15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" customFormat="1" spans="1:7">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" customFormat="1" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -3794,14 +3846,15 @@
       <c r="G16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" customFormat="1" spans="1:7">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" customFormat="1" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -3815,11 +3868,193 @@
       <c r="G17" t="s">
         <v>13</v>
       </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="19" customFormat="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" spans="1:8">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" customFormat="1" spans="1:8">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" customFormat="1" spans="1:8">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" customFormat="1" spans="1:8">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" customFormat="1" spans="1:8">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" customFormat="1" spans="1:8">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" customFormat="1" spans="1:8">
+      <c r="A26" s="4"/>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="H3:H10"/>
+    <mergeCell ref="H12:H17"/>
+    <mergeCell ref="H19:H26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3896,7 +4131,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -3917,7 +4152,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -3968,10 +4203,10 @@
         <v>12</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">
@@ -4045,7 +4280,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -4066,7 +4301,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:3">
@@ -4075,7 +4310,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:3">
@@ -4084,7 +4319,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:3">
@@ -4093,7 +4328,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:3">
@@ -4102,7 +4337,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="2:3">
@@ -4110,7 +4345,7 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4172,7 +4407,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -4193,7 +4428,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -4205,7 +4440,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:7">
@@ -4214,7 +4449,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -4235,7 +4470,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -4256,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -4265,10 +4500,10 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">
@@ -4277,7 +4512,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -4298,7 +4533,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -4319,7 +4554,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -4342,7 +4577,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -4360,7 +4595,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -4378,7 +4613,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -4396,7 +4631,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -4414,7 +4649,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -4432,7 +4667,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -4449,7 +4684,7 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -4520,7 +4755,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -4529,7 +4764,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:3">
@@ -4538,7 +4773,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
@@ -4547,7 +4782,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:3">
@@ -4556,7 +4791,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:3">
@@ -4565,7 +4800,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:3">
@@ -4574,7 +4809,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:3">
@@ -4583,7 +4818,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:3">
@@ -4594,7 +4829,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:3">
@@ -4603,7 +4838,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:3">
@@ -4612,7 +4847,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:3">
@@ -4621,7 +4856,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:3">
@@ -4630,7 +4865,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:3">
@@ -4639,7 +4874,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="2:3">
@@ -4647,12 +4882,12 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated class 6 second language poems
</commit_message>
<xml_diff>
--- a/TestReport1.xlsx
+++ b/TestReport1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="9000" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="11735" windowHeight="9000" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="181">
   <si>
     <t>Content</t>
   </si>
@@ -352,61 +352,61 @@
     <t>Nee hada marudina</t>
   </si>
   <si>
-    <t>No</t>
+    <t>IR 1.0 fix</t>
+  </si>
+  <si>
+    <t>ee mannu nammadu</t>
+  </si>
+  <si>
+    <t>nanna desha nanna jana</t>
+  </si>
+  <si>
+    <t>nammura kere</t>
+  </si>
+  <si>
+    <t>kannadamma</t>
+  </si>
+  <si>
+    <t>aikyagaana</t>
+  </si>
+  <si>
+    <t>suntaragaali</t>
+  </si>
+  <si>
+    <t>chutukugalu</t>
+  </si>
+  <si>
+    <t>The Rainbow</t>
+  </si>
+  <si>
+    <t>Sympathy</t>
+  </si>
+  <si>
+    <t>Kindness to animals</t>
+  </si>
+  <si>
+    <t>All things bright and beautiful</t>
+  </si>
+  <si>
+    <t>The Fly</t>
+  </si>
+  <si>
+    <t>The way to succeed</t>
+  </si>
+  <si>
+    <t>My people</t>
+  </si>
+  <si>
+    <t>A sonnet for my incomparable mother</t>
+  </si>
+  <si>
+    <t>Huttari haadu</t>
+  </si>
+  <si>
+    <t>Swathanthrya swarga</t>
   </si>
   <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>ee mannu nammadu</t>
-  </si>
-  <si>
-    <t>nanna desha nanna jana</t>
-  </si>
-  <si>
-    <t>nammura kere</t>
-  </si>
-  <si>
-    <t>kannadamma</t>
-  </si>
-  <si>
-    <t>aikyagaana</t>
-  </si>
-  <si>
-    <t>suntaragaali</t>
-  </si>
-  <si>
-    <t>chutukugalu</t>
-  </si>
-  <si>
-    <t>The Rainbow</t>
-  </si>
-  <si>
-    <t>Sympathy</t>
-  </si>
-  <si>
-    <t>Kindness to animals</t>
-  </si>
-  <si>
-    <t>All things bright and beautiful</t>
-  </si>
-  <si>
-    <t>The Fly</t>
-  </si>
-  <si>
-    <t>The way to succeed</t>
-  </si>
-  <si>
-    <t>My people</t>
-  </si>
-  <si>
-    <t>A sonnet for my incomparable mother</t>
-  </si>
-  <si>
-    <t>Huttari haadu</t>
-  </si>
-  <si>
-    <t>Swathanthrya swarga</t>
   </si>
   <si>
     <t>bhagyaada balegaara</t>
@@ -3545,8 +3545,8 @@
   <sheetPr/>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="$A19:$XFD26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -3631,22 +3631,22 @@
     </row>
     <row r="5" customFormat="1" spans="1:8">
       <c r="A5" s="4"/>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="6"/>
@@ -3682,13 +3682,16 @@
         <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
       </c>
       <c r="H7" s="6"/>
     </row>
@@ -4090,8 +4093,8 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C27"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4212,7 +4215,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="1" spans="1:7">
+    <row r="7" customFormat="1" spans="1:8">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>20</v>
@@ -4227,10 +4230,13 @@
         <v>12</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
         <v>104</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">
@@ -4304,7 +4310,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -4325,7 +4331,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:3">
@@ -4334,7 +4340,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:3">
@@ -4343,7 +4349,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:3">
@@ -4352,7 +4358,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:3">
@@ -4361,7 +4367,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="2:3">
@@ -4369,7 +4375,7 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:8">
@@ -4380,7 +4386,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -4404,7 +4410,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>22</v>
@@ -4426,7 +4432,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -4448,7 +4454,7 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -4470,7 +4476,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -4492,7 +4498,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -4514,7 +4520,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>22</v>
@@ -4536,7 +4542,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>22</v>
@@ -4613,7 +4619,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -4634,19 +4640,19 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
         <v>122</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:7">
@@ -4709,7 +4715,7 @@
         <v>126</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">

</xml_diff>

<commit_message>
Updated class 6 poems
</commit_message>
<xml_diff>
--- a/TestReport1.xlsx
+++ b/TestReport1.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="181">
   <si>
     <t>Content</t>
   </si>
@@ -3546,7 +3546,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4093,8 +4093,8 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4325,7 +4325,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:3">
+    <row r="13" customFormat="1" spans="1:7">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>14</v>
@@ -4333,8 +4333,20 @@
       <c r="C13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" customFormat="1" spans="1:3">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" spans="1:7">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>16</v>
@@ -4342,8 +4354,20 @@
       <c r="C14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" customFormat="1" spans="1:3">
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:7">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>18</v>
@@ -4351,8 +4375,20 @@
       <c r="C15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" customFormat="1" spans="1:3">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" spans="1:7">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>20</v>
@@ -4360,8 +4396,20 @@
       <c r="C16" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" customFormat="1" spans="1:3">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:7">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>23</v>
@@ -4369,13 +4417,37 @@
       <c r="C17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="2:3">
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:8">

</xml_diff>

<commit_message>
Updated call 7 english poems
</commit_message>
<xml_diff>
--- a/TestReport1.xlsx
+++ b/TestReport1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11735" windowHeight="9000" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="11520" windowHeight="9000" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="189">
   <si>
     <t>Content</t>
   </si>
@@ -449,6 +449,30 @@
   </si>
   <si>
     <t>sarvajnana vachanagalu</t>
+  </si>
+  <si>
+    <t>The gymnastic clock</t>
+  </si>
+  <si>
+    <t>Awareness</t>
+  </si>
+  <si>
+    <t>Why god made Teachers</t>
+  </si>
+  <si>
+    <t>Froth and Bubble</t>
+  </si>
+  <si>
+    <t>Abou Ben Adhem leigh hunt</t>
+  </si>
+  <si>
+    <t>Mountain climbing Laura howell Horner</t>
+  </si>
+  <si>
+    <t>Dear Grandma and Grandpa</t>
+  </si>
+  <si>
+    <t>The Quarrel</t>
   </si>
   <si>
     <t>kannadigara thaayi</t>
@@ -1238,11 +1262,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2062,7 +2086,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -2071,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:3">
@@ -2080,7 +2104,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
@@ -2089,7 +2113,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:3">
@@ -2098,7 +2122,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:3">
@@ -2107,7 +2131,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:3">
@@ -2116,7 +2140,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:3">
@@ -2125,7 +2149,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:3">
@@ -2136,7 +2160,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:3">
@@ -2145,7 +2169,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:3">
@@ -2154,7 +2178,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:3">
@@ -2163,7 +2187,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:3">
@@ -2172,7 +2196,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:3">
@@ -2181,7 +2205,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="2:3">
@@ -2194,7 +2218,7 @@
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2372,56 +2396,56 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="34.8" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" ht="27.6" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E4" s="2">
         <v>2.1</v>
@@ -2432,7 +2456,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3603,7 +3627,7 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3627,29 +3651,29 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" customFormat="1" spans="1:8">
       <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" customFormat="1" spans="1:8">
       <c r="A6" s="4"/>
@@ -3671,7 +3695,7 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="1" spans="1:8">
       <c r="A7" s="4"/>
@@ -3693,7 +3717,7 @@
       <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="1" spans="1:8">
       <c r="A8" s="4"/>
@@ -3715,7 +3739,7 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="1" spans="1:8">
       <c r="A9" s="4"/>
@@ -3737,7 +3761,7 @@
       <c r="G9" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="1" spans="1:8">
       <c r="A10" s="4"/>
@@ -3759,7 +3783,7 @@
       <c r="G10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="12" customFormat="1" spans="1:8">
       <c r="A12" s="4" t="s">
@@ -3783,7 +3807,7 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3807,7 +3831,7 @@
       <c r="G13" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="1" spans="1:8">
       <c r="A14" s="4"/>
@@ -3829,7 +3853,7 @@
       <c r="G14" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" customFormat="1" spans="1:8">
       <c r="A15" s="4"/>
@@ -3851,7 +3875,7 @@
       <c r="G15" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" customFormat="1" spans="1:8">
       <c r="A16" s="4"/>
@@ -3873,7 +3897,7 @@
       <c r="G16" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" customFormat="1" spans="1:8">
       <c r="A17" s="4"/>
@@ -3895,7 +3919,7 @@
       <c r="G17" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="19" customFormat="1" spans="1:8">
       <c r="A19" s="4" t="s">
@@ -3919,7 +3943,7 @@
       <c r="G19" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3943,7 +3967,7 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" customFormat="1" spans="1:8">
       <c r="A21" s="4"/>
@@ -3965,29 +3989,29 @@
       <c r="G21" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" customFormat="1" spans="1:8">
       <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" customFormat="1" spans="1:8">
       <c r="A23" s="4"/>
@@ -4006,7 +4030,7 @@
       <c r="F23" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" customFormat="1" spans="1:8">
       <c r="A24" s="4"/>
@@ -4028,29 +4052,29 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" customFormat="1" spans="1:8">
       <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" customFormat="1" spans="1:8">
       <c r="A26" s="4"/>
@@ -4072,7 +4096,7 @@
       <c r="G26" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4093,8 +4117,8 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B20" sqref="$A20:$XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4220,19 +4244,19 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H7" t="s">
@@ -4376,7 +4400,7 @@
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -4397,7 +4421,7 @@
         <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -4472,31 +4496,31 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="1:8">
       <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" customFormat="1" spans="1:8">
       <c r="A22" s="4"/>
@@ -4518,7 +4542,7 @@
       <c r="G22" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" customFormat="1" spans="1:8">
       <c r="A23" s="4"/>
@@ -4540,7 +4564,7 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" customFormat="1" spans="1:8">
       <c r="A24" s="4"/>
@@ -4562,7 +4586,7 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" customFormat="1" spans="1:8">
       <c r="A25" s="4"/>
@@ -4584,51 +4608,51 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" customFormat="1" spans="1:8">
       <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" customFormat="1" spans="1:8">
       <c r="A27" s="4"/>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4645,10 +4669,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.287037037037" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4980,10 +5004,192 @@
         <v>11</v>
       </c>
     </row>
+    <row r="20" customFormat="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" customFormat="1" spans="1:8">
+      <c r="A21" s="4"/>
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" customFormat="1" spans="1:8">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" customFormat="1" spans="1:8">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" customFormat="1" spans="1:8">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" customFormat="1" spans="1:8">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" customFormat="1" spans="1:8">
+      <c r="A26" s="4"/>
+      <c r="B26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" customFormat="1" spans="1:8">
+      <c r="A27" s="4"/>
+      <c r="B27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="H20:H27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -5039,7 +5245,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -5048,7 +5254,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:3">
@@ -5057,7 +5263,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
@@ -5066,7 +5272,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:3">
@@ -5075,7 +5281,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:3">
@@ -5084,7 +5290,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:3">
@@ -5093,7 +5299,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:3">
@@ -5102,7 +5308,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:3">
@@ -5113,7 +5319,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:3">
@@ -5122,7 +5328,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:3">
@@ -5131,7 +5337,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:3">
@@ -5140,7 +5346,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:3">
@@ -5149,7 +5355,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:3">
@@ -5158,7 +5364,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="2:3">
@@ -5166,12 +5372,12 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pdf render issue - bug fix testing
</commit_message>
<xml_diff>
--- a/TestReport1.xlsx
+++ b/TestReport1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="9000" firstSheet="4" activeTab="7"/>
+    <workbookView windowWidth="11520" windowHeight="9000" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="190">
   <si>
     <t>Content</t>
   </si>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>#1002</t>
+  </si>
+  <si>
+    <t>pdf's are not displayed unless the page is refreshed atleast once</t>
   </si>
 </sst>
 </file>
@@ -2380,8 +2383,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -2454,9 +2457,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>188</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4671,7 +4689,7 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>

</xml_diff>